<commit_message>
Uploaded the right branch
</commit_message>
<xml_diff>
--- a/public/templates/student_template.xlsx
+++ b/public/templates/student_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17720" windowHeight="9560"/>
+    <workbookView windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,49 +29,49 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>lrn</t>
-  </si>
-  <si>
-    <t>student_id</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>middle_name</t>
-  </si>
-  <si>
-    <t>birth_date</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>contact_number</t>
-  </si>
-  <si>
-    <t>guardian_name</t>
-  </si>
-  <si>
-    <t>guardian_contact</t>
-  </si>
-  <si>
-    <t>grade_level</t>
-  </si>
-  <si>
-    <t>section_name</t>
-  </si>
-  <si>
-    <t>school_year</t>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>LRN</t>
+  </si>
+  <si>
+    <t>STUDENT ID</t>
+  </si>
+  <si>
+    <t>FIRST NAME</t>
+  </si>
+  <si>
+    <t>LAST NAME</t>
+  </si>
+  <si>
+    <t>MIDDLE NAME</t>
+  </si>
+  <si>
+    <t>BIRTH DATE</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>CONTACT NUMBER</t>
+  </si>
+  <si>
+    <t>GUARDIAN NAME</t>
+  </si>
+  <si>
+    <t>GUARDIAN CONTACT</t>
+  </si>
+  <si>
+    <t>GRADE LEVEL</t>
+  </si>
+  <si>
+    <t>SECTION NAME</t>
+  </si>
+  <si>
+    <t>SCHOOL YEAR</t>
   </si>
 </sst>
 </file>
@@ -80,15 +80,23 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -445,12 +453,64 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -554,159 +614,171 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1186,12 +1258,25 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A$1:A$1048576"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="2"/>
   <cols>
-    <col min="2" max="2" width="12.7857142857143"/>
+    <col min="1" max="1" width="14.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="16.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="15.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="15.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="15.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="15.2857142857143" customWidth="1"/>
+    <col min="8" max="8" width="15.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="13.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="19.1428571428571" customWidth="1"/>
+    <col min="11" max="11" width="18.5714285714286" customWidth="1"/>
+    <col min="12" max="12" width="20.4285714285714" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="15" width="17.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:15">
@@ -1210,72 +1295,72 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:16">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" customHeight="1" spans="1:16">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>